<commit_message>
Upload fichier data_files/unit data.xlsx
</commit_message>
<xml_diff>
--- a/data_files/unit data.xlsx
+++ b/data_files/unit data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\ULB\Passerelle\INFO-H304 Compléments de programmation et d_algorithmique\Projet\advance-wars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\ULB\Passerelle\INFO-H304 Compléments de programmation et d_algorithmique\Projet\advance-wars\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8AF04B-8062-4327-96AD-110E0909CBA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7ADB0-23E3-4403-998A-10E54339127D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5004" xr2:uid="{7543C2BC-01CB-4C68-9E9C-98582548CE7F}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>Unit</t>
   </si>
@@ -624,7 +624,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,9 +674,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>